<commit_message>
Hobo temp graphs, updating current frag status
</commit_message>
<xml_diff>
--- a/lab/data_raw/Cycle monitoring.xlsx
+++ b/lab/data_raw/Cycle monitoring.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>(Ernesto)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2ml of amonium chloride added </t>
+  </si>
+  <si>
+    <t>MWW/GRB</t>
   </si>
 </sst>
 </file>
@@ -1021,6 +1027,12 @@
       <c r="C20" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="G20" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="3">
@@ -1030,6 +1042,215 @@
         <v>20.0</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="4">
+        <v>8.22</v>
+      </c>
+      <c r="F21" s="4">
+        <v>37.9</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="I21" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3">
+        <v>45521.0</v>
+      </c>
+      <c r="B22" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="4">
+        <v>38.2</v>
+      </c>
+      <c r="G22" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="I22" s="4">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3">
+        <v>45522.0</v>
+      </c>
+      <c r="B23" s="4">
+        <v>22.0</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="4">
+        <v>38.9</v>
+      </c>
+      <c r="G23" s="4">
+        <v>0.06</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="I23" s="4">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3">
+        <v>45523.0</v>
+      </c>
+      <c r="B24" s="4">
+        <v>23.0</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="4">
+        <v>39.3</v>
+      </c>
+      <c r="G24" s="4">
+        <v>0.06</v>
+      </c>
+      <c r="H24" s="4">
+        <v>0.35</v>
+      </c>
+      <c r="I24" s="4">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3">
+        <v>45524.0</v>
+      </c>
+      <c r="B25" s="4">
+        <v>24.0</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="4">
+        <v>40.2</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="H25" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="I25" s="4">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3">
+        <v>45525.0</v>
+      </c>
+      <c r="B26" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="4">
+        <v>8.22</v>
+      </c>
+      <c r="F26" s="4">
+        <v>41.8</v>
+      </c>
+      <c r="G26" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="H26" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="I26" s="4">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3">
+        <v>45526.0</v>
+      </c>
+      <c r="B27" s="4">
+        <v>26.0</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3">
+        <v>45527.0</v>
+      </c>
+      <c r="B28" s="4">
+        <v>27.0</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3">
+        <v>45528.0</v>
+      </c>
+      <c r="B29" s="4">
+        <v>28.0</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3">
+        <v>45529.0</v>
+      </c>
+      <c r="B30" s="4">
+        <v>29.0</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="3">
+        <v>45530.0</v>
+      </c>
+      <c r="B31" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>